<commit_message>
Deploy til rot: LMDI - 73b16c85ec256fca8e1394087d930635a0f9fd81
</commit_message>
<xml_diff>
--- a/CodeSystem-LokalLegemiddelkatalogCodeSystem.xlsx
+++ b/CodeSystem-LokalLegemiddelkatalogCodeSystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0</t>
+    <t>1.0.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-03-24T12:30:17+00:00</t>
+    <t>2025-03-25T12:34:21+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Deploy til rot: LMDI - 0b5da222a960e59e4d66c5d1267b541540fffede
</commit_message>
<xml_diff>
--- a/CodeSystem-LokalLegemiddelkatalogCodeSystem.xlsx
+++ b/CodeSystem-LokalLegemiddelkatalogCodeSystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.1</t>
+    <t>1.0.2</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-03-25T12:47:44+00:00</t>
+    <t>2025-03-31T14:08:18+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Deploy til rot: LMDI - 9336ef494ea8b5abef60ab5eac47b2a391996be5
</commit_message>
<xml_diff>
--- a/CodeSystem-LokalLegemiddelkatalogCodeSystem.xlsx
+++ b/CodeSystem-LokalLegemiddelkatalogCodeSystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.2</t>
+    <t>1.0.3</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-03-31T14:08:18+00:00</t>
+    <t>2025-04-11T07:26:01+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Deploy til rot: LMDI - 5ef8a69f44a90501673d81afcb2f7bdd2d7082bb
</commit_message>
<xml_diff>
--- a/CodeSystem-LokalLegemiddelkatalogCodeSystem.xlsx
+++ b/CodeSystem-LokalLegemiddelkatalogCodeSystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.3</t>
+    <t>1.0.4</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-04-11T07:26:01+00:00</t>
+    <t>2025-08-29T09:13:21+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>